<commit_message>
Add product type and accessory
</commit_message>
<xml_diff>
--- a/furniture_v2_be/src/UploadFiles/product.xlsx
+++ b/furniture_v2_be/src/UploadFiles/product.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1314F658-9ED7-4156-B6A2-0175751702FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC14B512-F142-4223-B7ED-0FD744A985BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,45 +26,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>sl đã bán</t>
-  </si>
-  <si>
-    <t>số % giảm</t>
-  </si>
-  <si>
-    <t>giá</t>
-  </si>
-  <si>
-    <t>trạng thái</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size </t>
-  </si>
-  <si>
-    <t>trọng lượng</t>
-  </si>
-  <si>
-    <t>trọng tải tối đa</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>SL đã bán</t>
+  </si>
+  <si>
+    <t>Số % giảm</t>
+  </si>
+  <si>
+    <t>Giá</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Loại sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size </t>
+  </si>
+  <si>
+    <t>Trọng lượng</t>
+  </si>
+  <si>
+    <t>Trọng tải tối đa</t>
   </si>
   <si>
     <t>Chức năng</t>
   </si>
   <si>
-    <t>hình ảnh</t>
-  </si>
-  <si>
-    <t>danh mục</t>
+    <t>Hình ảnh</t>
+  </si>
+  <si>
+    <t>Danh mục</t>
   </si>
   <si>
     <t>Ergonomic chair</t>
@@ -446,18 +449,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:P3"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" ht="24" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,10 +487,10 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M1" t="s">
@@ -497,13 +505,16 @@
       <c r="P1" t="s">
         <v>12</v>
       </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>15</v>
@@ -520,25 +531,28 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>150</v>
       </c>
-      <c r="N2" t="s">
-        <v>16</v>
+      <c r="O2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -555,17 +569,20 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3">
         <v>70</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>400</v>
       </c>
-      <c r="N3" t="s">
-        <v>20</v>
+      <c r="O3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>